<commit_message>
aktuelles Tagebuch + Namen geändert
</commit_message>
<xml_diff>
--- a/dev-diaries/diary-person-1.xlsx
+++ b/dev-diaries/diary-person-1.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\friedrich\Projekte\dlvc\vorlagen\content\dev-diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\development\group-1\dev-diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845F9A7E-DA74-4CE3-A6BD-46C9DEDBA294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="38" windowWidth="15960" windowHeight="17348" activeTab="1"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diary" sheetId="1" r:id="rId1"/>
     <sheet name="Reflection" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -49,13 +63,7 @@
     <t>Beitrag zum Projekt</t>
   </si>
   <si>
-    <t>Erste Infoveranstaltung - Einführung in das Projekt und Vorstellung der Teams sowie erste grobe Einteilung</t>
-  </si>
-  <si>
     <t>Ablauf, Organisatorisches, Projektziel, Vorstellung der Themen</t>
-  </si>
-  <si>
-    <t>Max Muster</t>
   </si>
   <si>
     <t>Gesamtzeit (bei 8 ECTS):</t>
@@ -76,9 +84,6 @@
     <t>Zeitaufwand in Dreiviertelstunden</t>
   </si>
   <si>
-    <t>Team X</t>
-  </si>
-  <si>
     <t>Team-Mitglied</t>
   </si>
   <si>
@@ -96,12 +101,90 @@
   <si>
     <t>w</t>
   </si>
+  <si>
+    <t>Erste Infoveranstaltung - Einführung in das Projekt und Vorstellung der Teams sowie erste grobe Einteilung.</t>
+  </si>
+  <si>
+    <t>KW 12</t>
+  </si>
+  <si>
+    <t>Aktuelle Bücher und Videos zum Thema vorgeschlagen. Richtung der Projektarbeit diskutiert. Aktuellen Stand zu den erarbeiteten Themen geteilt. Idee: GRAD-CAM als neuen Algorithmus später in GUI hinzuzufügen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustering Algorithmen Matrix und Repräsentationsschemas. Prinzipien und Ideen hinter verschiedenen Algorithmen. Wichtigkeit und Motivation von Explainable AI. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einarbeitung in Thema: - Integrated Gradients + weitere Algorithmen + Papers lesen. Aufsetzen der Captum GUI und Ausführen aller Algorithmen. Ausführen einiger Algorithmen in PyCharm. Besprechung der Inhalte und Aufgabenaufteilung mit Teamkollegen. </t>
+  </si>
+  <si>
+    <t>KW 13</t>
+  </si>
+  <si>
+    <t>KW 14</t>
+  </si>
+  <si>
+    <t>KW 15</t>
+  </si>
+  <si>
+    <t>KW 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paper Präsentation vorbereitet. Ausarbeitung der Stichpunkte in den Präsentationsfolien. Hinzufügen von passenden Bildern (+ Quellenangaben). Für meinen Teil der Paperpräsentation habe ich die Folien deutlich reduziert von 8 auf 3, um die 5 Minuten Vortragszeit einzuhalten. Ich habe speziell die Folieninhalte zu Einleitung, Saliency Maps, TCAV und Ziele gestaltet. Feedback und Unterstützung bei der Formulierung der Folien zur Validierung von TCAV und Präsentations- und Änderungsvorschläge für den Code Teil gegeben. </t>
+  </si>
+  <si>
+    <t>11.04.2023 (Ostern)</t>
+  </si>
+  <si>
+    <t>Einarbeitung in die Funktionsweise von verschiedenen Algorithmen auf Captum. TCAV Paper gelesen und Videos zur funktionsweise angeschaut. Überblick zu den verschiedenen Algorithmen in Captum  bekommen. Austausch mit der Gruppe zu den Möglichkeiten Captum einzusetzen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Präsentationsfüllen mit groben Stichpunkten befüllt und Reihenfolge der Inhalten vorgegeben. </t>
+  </si>
+  <si>
+    <t>TCAV wiederholt und versucht die Schritte nachzuvollziehen.</t>
+  </si>
+  <si>
+    <t>Babar Ayan</t>
+  </si>
+  <si>
+    <t>Team 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idee hinter mathematische Erklärung und Validierung von TCAV verstanden. </t>
+  </si>
+  <si>
+    <t>Über funktionsweise von TCAV mit der Gruppe ausgetauscht</t>
+  </si>
+  <si>
+    <t>Gliederung der Präsentation</t>
+  </si>
+  <si>
+    <t>Folien für Paperpräsentation erstellt und die Gruppe unterstützt mit Vorschlägen.</t>
+  </si>
+  <si>
+    <t>GradCAM Paper gelesen und grob über Funktionsweise recherchiert</t>
+  </si>
+  <si>
+    <t>Austausch mit der Gruppe über die Funktionsweise von Captum.</t>
+  </si>
+  <si>
+    <t>Nutzung von Stride anstatt Pooling. Bedienung von Captum GUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCAV verständnis nochmal vertieft durch die Erstellung der Präsentationsfolien, Transfer Learning, </t>
+  </si>
+  <si>
+    <t>Fortgeschrittene Architekturen in Deep Learning, speziell ResNets und Positional Encoding bei Transformers + Nutzung von Transformers anstatt CNNs für Bildklassifikation.</t>
+  </si>
+  <si>
+    <t>Feature Visualisierung und Nachteile von Saliency Maps.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -145,8 +228,106 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,8 +346,50 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFCC0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -240,23 +463,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="4">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="7">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4">
+      <alignment wrapText="1"/>
+    </xf>
+  </cellStyleXfs>
+  <cellXfs count="28">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -265,67 +575,92 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="20">
+    <cellStyle name="Accent" xfId="3" xr:uid="{3D67A071-3F6C-485D-95CC-D2DD8E73FF98}"/>
+    <cellStyle name="Accent 1" xfId="4" xr:uid="{0967D2A0-43E8-497C-87C9-059FBC3ABDE7}"/>
+    <cellStyle name="Accent 2" xfId="5" xr:uid="{46D1BBD8-5F38-4A3B-8E53-83CA7EDF1E5C}"/>
+    <cellStyle name="Accent 3" xfId="6" xr:uid="{3B76952A-7572-43AC-9AE2-FE82512AADC4}"/>
+    <cellStyle name="Bad" xfId="7" xr:uid="{C0BBE2CA-6FCD-4F4B-B0AC-13584641BCAC}"/>
+    <cellStyle name="Error" xfId="8" xr:uid="{F4B35E58-ED67-467E-A289-9D7EA0503D6D}"/>
+    <cellStyle name="Footnote" xfId="9" xr:uid="{DA357EA7-0E47-4ACD-8461-C3CB645ED68F}"/>
+    <cellStyle name="Good" xfId="10" xr:uid="{6AB0D657-3E23-4CD0-B700-4CC590A0776D}"/>
+    <cellStyle name="Heading" xfId="11" xr:uid="{287F8694-D1E6-4C81-ACF8-0EA52431C519}"/>
+    <cellStyle name="Heading 1" xfId="12" xr:uid="{562EFDAA-9843-4160-8AFA-65C1B223CB77}"/>
+    <cellStyle name="Heading 2" xfId="13" xr:uid="{17F36163-7B1D-4B3F-9C70-AD3BE1A43F64}"/>
+    <cellStyle name="Hyperlink" xfId="14" xr:uid="{7F3607C0-5A1D-4221-B4EF-EAC04F9A17E0}"/>
+    <cellStyle name="Neutral 2" xfId="2" xr:uid="{A25CB44B-CDAA-4F8D-9FF4-0E1FB61339D9}"/>
+    <cellStyle name="Note" xfId="15" xr:uid="{F987A55E-BDA7-459B-819C-258D8DA6B989}"/>
+    <cellStyle name="Result" xfId="16" xr:uid="{B69898EC-B12C-4B75-86C7-DF58C28B51AF}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{060B43ED-89CA-4535-B802-A590918C3629}"/>
+    <cellStyle name="Status" xfId="17" xr:uid="{42F5CBE6-7FF6-4544-8E0D-6F6FF246BA0E}"/>
+    <cellStyle name="Text" xfId="18" xr:uid="{26E54490-37B7-4762-8892-9BADA4BACE1D}"/>
+    <cellStyle name="Warning" xfId="19" xr:uid="{73EBEF65-55D7-41C9-9702-CE6C9E1A1260}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -423,7 +758,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -486,6 +820,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8DB7-40A8-A151-A6FD3FD42FD7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -501,6 +840,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8DB7-40A8-A151-A6FD3FD42FD7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -516,6 +860,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-8DB7-40A8-A151-A6FD3FD42FD7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -531,6 +880,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8DB7-40A8-A151-A6FD3FD42FD7}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -600,7 +954,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1243,7 +1596,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2365,24 +2724,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q152"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.19921875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.19921875" style="1" customWidth="1"/>
-    <col min="3" max="6" width="35.86328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.19921875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.86328125" style="1" customWidth="1"/>
-    <col min="9" max="18" width="17.19921875" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="17.19921875" style="1"/>
+    <col min="1" max="2" width="17.140625" style="1" customWidth="1"/>
+    <col min="3" max="6" width="35.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" customWidth="1"/>
+    <col min="9" max="18" width="17.140625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="17.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2401,9 +2760,9 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2422,18 +2781,18 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -2449,12 +2808,12 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2472,7 +2831,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -2491,7 +2850,7 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
@@ -2504,7 +2863,7 @@
         <v>3</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -2516,7 +2875,7 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
@@ -2524,11 +2883,11 @@
       <c r="E7" s="4"/>
       <c r="F7" s="8">
         <f>SUM(F10:F152)</f>
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="G7" s="8">
         <f>H7-F7</f>
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="H7" s="8">
         <f>5*30</f>
@@ -2544,7 +2903,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -2563,7 +2922,7 @@
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
     </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
@@ -2580,7 +2939,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
@@ -2594,18 +2953,18 @@
       <c r="P9" s="15"/>
       <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="18">
-        <v>44475</v>
-      </c>
-      <c r="C10" s="17" t="s">
+        <v>45013</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>9</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>10</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="20">
@@ -2623,13 +2982,25 @@
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
     </row>
-    <row r="11" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+    <row r="11" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="18">
+        <v>45020</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="2">
+        <v>14</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -2642,13 +3013,25 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+    <row r="12" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="2">
+        <v>10</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -2661,13 +3044,25 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+    <row r="13" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="18">
+        <v>45034</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="2">
+        <v>12</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2680,13 +3075,25 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+    <row r="14" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="18">
+        <v>45041</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="2">
+        <v>8</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -2699,13 +3106,25 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="191.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+    <row r="15" spans="1:17" ht="191.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="18">
+        <v>45048</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="2">
+        <v>21</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -2718,13 +3137,21 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="18">
+        <v>45055</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>47</v>
+      </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2">
+        <v>6</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -2737,9 +3164,11 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="B17" s="18">
+        <v>45062</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -2756,7 +3185,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2775,7 +3204,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2794,7 +3223,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="5"/>
       <c r="C20" s="2"/>
@@ -2813,7 +3242,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="5"/>
       <c r="C21" s="2"/>
@@ -2832,7 +3261,7 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="5"/>
       <c r="C22" s="2"/>
@@ -2851,7 +3280,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="5"/>
       <c r="C23" s="2"/>
@@ -2870,7 +3299,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="5"/>
       <c r="C24" s="2"/>
@@ -2889,7 +3318,7 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
@@ -2908,7 +3337,7 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
     </row>
-    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="5"/>
       <c r="C26" s="2"/>
@@ -2927,7 +3356,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
       <c r="C27" s="2"/>
@@ -2946,7 +3375,7 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="5"/>
       <c r="C28" s="2"/>
@@ -2965,7 +3394,7 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
     </row>
-    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="5"/>
       <c r="C29" s="2"/>
@@ -2984,7 +3413,7 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="5"/>
       <c r="C30" s="2"/>
@@ -3003,7 +3432,7 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
     </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="5"/>
       <c r="C31" s="2"/>
@@ -3022,7 +3451,7 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="5"/>
       <c r="C32" s="2"/>
@@ -3041,7 +3470,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="5"/>
       <c r="C33" s="2"/>
@@ -3060,7 +3489,7 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
     </row>
-    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="5"/>
       <c r="C34" s="2"/>
@@ -3079,7 +3508,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="5"/>
       <c r="C35" s="2"/>
@@ -3098,7 +3527,7 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
     </row>
-    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="C36" s="2"/>
@@ -3117,7 +3546,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="5"/>
       <c r="C37" s="2"/>
@@ -3136,7 +3565,7 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="5"/>
       <c r="C38" s="2"/>
@@ -3155,7 +3584,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="5"/>
       <c r="C39" s="2"/>
@@ -3174,7 +3603,7 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
     </row>
-    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="5"/>
       <c r="C40" s="2"/>
@@ -3193,7 +3622,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="5"/>
       <c r="C41" s="2"/>
@@ -3212,7 +3641,7 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
-    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="5"/>
       <c r="C42" s="2"/>
@@ -3231,7 +3660,7 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
-    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="5"/>
       <c r="C43" s="2"/>
@@ -3250,7 +3679,7 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
-    <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="5"/>
       <c r="C44" s="2"/>
@@ -3269,7 +3698,7 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="C45" s="2"/>
@@ -3288,7 +3717,7 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="5"/>
       <c r="C46" s="2"/>
@@ -3307,7 +3736,7 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="5"/>
       <c r="C47" s="2"/>
@@ -3326,7 +3755,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="5"/>
       <c r="C48" s="2"/>
@@ -3345,7 +3774,7 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
-    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="5"/>
       <c r="C49" s="2"/>
@@ -3364,7 +3793,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="5"/>
       <c r="C50" s="2"/>
@@ -3383,7 +3812,7 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
     </row>
-    <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="5"/>
       <c r="C51" s="2"/>
@@ -3402,7 +3831,7 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
     </row>
-    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="5"/>
       <c r="C52" s="2"/>
@@ -3421,7 +3850,7 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
     </row>
-    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="5"/>
       <c r="C53" s="2"/>
@@ -3440,7 +3869,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
     </row>
-    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="5"/>
       <c r="C54" s="2"/>
@@ -3459,7 +3888,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
     </row>
-    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="5"/>
       <c r="C55" s="2"/>
@@ -3478,7 +3907,7 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
     </row>
-    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="5"/>
       <c r="C56" s="2"/>
@@ -3497,7 +3926,7 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
     </row>
-    <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="5"/>
       <c r="C57" s="2"/>
@@ -3516,7 +3945,7 @@
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
     </row>
-    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="5"/>
       <c r="C58" s="2"/>
@@ -3535,7 +3964,7 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
     </row>
-    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="5"/>
       <c r="C59" s="2"/>
@@ -3554,7 +3983,7 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
     </row>
-    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="5"/>
       <c r="C60" s="2"/>
@@ -3573,7 +4002,7 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
     </row>
-    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="5"/>
       <c r="C61" s="2"/>
@@ -3592,7 +4021,7 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
-    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="5"/>
       <c r="C62" s="2"/>
@@ -3611,7 +4040,7 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
     </row>
-    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="5"/>
       <c r="C63" s="2"/>
@@ -3630,7 +4059,7 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
     </row>
-    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="5"/>
       <c r="C64" s="2"/>
@@ -3649,7 +4078,7 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
     </row>
-    <row r="65" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="5"/>
       <c r="C65" s="2"/>
@@ -3668,7 +4097,7 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
     </row>
-    <row r="66" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="5"/>
       <c r="C66" s="2"/>
@@ -3687,7 +4116,7 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
     </row>
-    <row r="67" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="5"/>
       <c r="C67" s="2"/>
@@ -3706,7 +4135,7 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
     </row>
-    <row r="68" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="5"/>
       <c r="C68" s="2"/>
@@ -3725,7 +4154,7 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
     </row>
-    <row r="69" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="5"/>
       <c r="C69" s="2"/>
@@ -3744,7 +4173,7 @@
       <c r="P69" s="2"/>
       <c r="Q69" s="2"/>
     </row>
-    <row r="70" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="5"/>
       <c r="C70" s="2"/>
@@ -3763,7 +4192,7 @@
       <c r="P70" s="2"/>
       <c r="Q70" s="2"/>
     </row>
-    <row r="71" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="5"/>
       <c r="C71" s="2"/>
@@ -3782,7 +4211,7 @@
       <c r="P71" s="2"/>
       <c r="Q71" s="2"/>
     </row>
-    <row r="72" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="5"/>
       <c r="C72" s="2"/>
@@ -3801,7 +4230,7 @@
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
     </row>
-    <row r="73" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="5"/>
       <c r="C73" s="2"/>
@@ -3820,7 +4249,7 @@
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
     </row>
-    <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="5"/>
       <c r="C74" s="2"/>
@@ -3839,7 +4268,7 @@
       <c r="P74" s="2"/>
       <c r="Q74" s="2"/>
     </row>
-    <row r="75" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="5"/>
       <c r="C75" s="2"/>
@@ -3858,7 +4287,7 @@
       <c r="P75" s="2"/>
       <c r="Q75" s="2"/>
     </row>
-    <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="5"/>
       <c r="C76" s="2"/>
@@ -3877,7 +4306,7 @@
       <c r="P76" s="2"/>
       <c r="Q76" s="2"/>
     </row>
-    <row r="77" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="5"/>
       <c r="C77" s="2"/>
@@ -3896,7 +4325,7 @@
       <c r="P77" s="2"/>
       <c r="Q77" s="2"/>
     </row>
-    <row r="78" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="5"/>
       <c r="C78" s="2"/>
@@ -3915,7 +4344,7 @@
       <c r="P78" s="2"/>
       <c r="Q78" s="2"/>
     </row>
-    <row r="79" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="5"/>
       <c r="C79" s="2"/>
@@ -3934,7 +4363,7 @@
       <c r="P79" s="2"/>
       <c r="Q79" s="2"/>
     </row>
-    <row r="80" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="5"/>
       <c r="C80" s="2"/>
@@ -3953,7 +4382,7 @@
       <c r="P80" s="2"/>
       <c r="Q80" s="2"/>
     </row>
-    <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="5"/>
       <c r="C81" s="2"/>
@@ -3972,7 +4401,7 @@
       <c r="P81" s="2"/>
       <c r="Q81" s="2"/>
     </row>
-    <row r="82" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="5"/>
       <c r="C82" s="2"/>
@@ -3991,7 +4420,7 @@
       <c r="P82" s="2"/>
       <c r="Q82" s="2"/>
     </row>
-    <row r="83" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="5"/>
       <c r="C83" s="2"/>
@@ -4010,7 +4439,7 @@
       <c r="P83" s="2"/>
       <c r="Q83" s="2"/>
     </row>
-    <row r="84" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="5"/>
       <c r="C84" s="2"/>
@@ -4029,7 +4458,7 @@
       <c r="P84" s="2"/>
       <c r="Q84" s="2"/>
     </row>
-    <row r="85" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="5"/>
       <c r="C85" s="2"/>
@@ -4048,7 +4477,7 @@
       <c r="P85" s="2"/>
       <c r="Q85" s="2"/>
     </row>
-    <row r="86" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="5"/>
       <c r="C86" s="2"/>
@@ -4067,7 +4496,7 @@
       <c r="P86" s="2"/>
       <c r="Q86" s="2"/>
     </row>
-    <row r="87" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="5"/>
       <c r="C87" s="2"/>
@@ -4086,7 +4515,7 @@
       <c r="P87" s="2"/>
       <c r="Q87" s="2"/>
     </row>
-    <row r="88" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="5"/>
       <c r="C88" s="2"/>
@@ -4105,7 +4534,7 @@
       <c r="P88" s="2"/>
       <c r="Q88" s="2"/>
     </row>
-    <row r="89" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="5"/>
       <c r="C89" s="2"/>
@@ -4124,7 +4553,7 @@
       <c r="P89" s="2"/>
       <c r="Q89" s="2"/>
     </row>
-    <row r="90" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="5"/>
       <c r="C90" s="2"/>
@@ -4143,7 +4572,7 @@
       <c r="P90" s="2"/>
       <c r="Q90" s="2"/>
     </row>
-    <row r="91" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="5"/>
       <c r="C91" s="2"/>
@@ -4162,7 +4591,7 @@
       <c r="P91" s="2"/>
       <c r="Q91" s="2"/>
     </row>
-    <row r="92" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="5"/>
       <c r="C92" s="2"/>
@@ -4181,7 +4610,7 @@
       <c r="P92" s="2"/>
       <c r="Q92" s="2"/>
     </row>
-    <row r="93" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="5"/>
       <c r="C93" s="2"/>
@@ -4200,7 +4629,7 @@
       <c r="P93" s="2"/>
       <c r="Q93" s="2"/>
     </row>
-    <row r="94" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="5"/>
       <c r="C94" s="2"/>
@@ -4219,7 +4648,7 @@
       <c r="P94" s="2"/>
       <c r="Q94" s="2"/>
     </row>
-    <row r="95" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="5"/>
       <c r="C95" s="2"/>
@@ -4238,7 +4667,7 @@
       <c r="P95" s="2"/>
       <c r="Q95" s="2"/>
     </row>
-    <row r="96" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="5"/>
       <c r="C96" s="2"/>
@@ -4257,7 +4686,7 @@
       <c r="P96" s="2"/>
       <c r="Q96" s="2"/>
     </row>
-    <row r="97" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="5"/>
       <c r="C97" s="2"/>
@@ -4276,7 +4705,7 @@
       <c r="P97" s="2"/>
       <c r="Q97" s="2"/>
     </row>
-    <row r="98" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="5"/>
       <c r="C98" s="2"/>
@@ -4295,7 +4724,7 @@
       <c r="P98" s="2"/>
       <c r="Q98" s="2"/>
     </row>
-    <row r="99" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="5"/>
       <c r="C99" s="2"/>
@@ -4314,7 +4743,7 @@
       <c r="P99" s="2"/>
       <c r="Q99" s="2"/>
     </row>
-    <row r="100" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="5"/>
       <c r="C100" s="2"/>
@@ -4333,7 +4762,7 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="5"/>
       <c r="C101" s="2"/>
@@ -4352,7 +4781,7 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="5"/>
       <c r="C102" s="2"/>
@@ -4371,7 +4800,7 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="5"/>
       <c r="C103" s="2"/>
@@ -4390,7 +4819,7 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="5"/>
       <c r="C104" s="2"/>
@@ -4409,7 +4838,7 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="5"/>
       <c r="C105" s="2"/>
@@ -4428,7 +4857,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -4447,7 +4876,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -4466,7 +4895,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -4485,7 +4914,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -4504,7 +4933,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -4523,7 +4952,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -4542,7 +4971,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -4561,7 +4990,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -4580,7 +5009,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -4599,7 +5028,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -4618,7 +5047,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -4637,7 +5066,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -4656,7 +5085,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -4675,7 +5104,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -4694,7 +5123,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -4713,7 +5142,7 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -4732,7 +5161,7 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -4751,7 +5180,7 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -4770,7 +5199,7 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -4789,7 +5218,7 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -4808,7 +5237,7 @@
       <c r="P125" s="2"/>
       <c r="Q125" s="2"/>
     </row>
-    <row r="126" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -4827,7 +5256,7 @@
       <c r="P126" s="2"/>
       <c r="Q126" s="2"/>
     </row>
-    <row r="127" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -4846,7 +5275,7 @@
       <c r="P127" s="2"/>
       <c r="Q127" s="2"/>
     </row>
-    <row r="128" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -4865,7 +5294,7 @@
       <c r="P128" s="2"/>
       <c r="Q128" s="2"/>
     </row>
-    <row r="129" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -4884,7 +5313,7 @@
       <c r="P129" s="2"/>
       <c r="Q129" s="2"/>
     </row>
-    <row r="130" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -4903,7 +5332,7 @@
       <c r="P130" s="2"/>
       <c r="Q130" s="2"/>
     </row>
-    <row r="131" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -4922,7 +5351,7 @@
       <c r="P131" s="2"/>
       <c r="Q131" s="2"/>
     </row>
-    <row r="132" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -4941,7 +5370,7 @@
       <c r="P132" s="2"/>
       <c r="Q132" s="2"/>
     </row>
-    <row r="133" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -4960,7 +5389,7 @@
       <c r="P133" s="2"/>
       <c r="Q133" s="2"/>
     </row>
-    <row r="134" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -4979,7 +5408,7 @@
       <c r="P134" s="2"/>
       <c r="Q134" s="2"/>
     </row>
-    <row r="135" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -4998,7 +5427,7 @@
       <c r="P135" s="2"/>
       <c r="Q135" s="2"/>
     </row>
-    <row r="136" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -5017,7 +5446,7 @@
       <c r="P136" s="2"/>
       <c r="Q136" s="2"/>
     </row>
-    <row r="137" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -5036,7 +5465,7 @@
       <c r="P137" s="2"/>
       <c r="Q137" s="2"/>
     </row>
-    <row r="138" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -5055,7 +5484,7 @@
       <c r="P138" s="2"/>
       <c r="Q138" s="2"/>
     </row>
-    <row r="139" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -5074,7 +5503,7 @@
       <c r="P139" s="2"/>
       <c r="Q139" s="2"/>
     </row>
-    <row r="140" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -5093,7 +5522,7 @@
       <c r="P140" s="2"/>
       <c r="Q140" s="2"/>
     </row>
-    <row r="141" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -5112,7 +5541,7 @@
       <c r="P141" s="2"/>
       <c r="Q141" s="2"/>
     </row>
-    <row r="142" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -5131,7 +5560,7 @@
       <c r="P142" s="2"/>
       <c r="Q142" s="2"/>
     </row>
-    <row r="143" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -5150,7 +5579,7 @@
       <c r="P143" s="2"/>
       <c r="Q143" s="2"/>
     </row>
-    <row r="144" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -5169,7 +5598,7 @@
       <c r="P144" s="2"/>
       <c r="Q144" s="2"/>
     </row>
-    <row r="145" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -5188,7 +5617,7 @@
       <c r="P145" s="2"/>
       <c r="Q145" s="2"/>
     </row>
-    <row r="146" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -5207,7 +5636,7 @@
       <c r="P146" s="2"/>
       <c r="Q146" s="2"/>
     </row>
-    <row r="147" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -5226,7 +5655,7 @@
       <c r="P147" s="2"/>
       <c r="Q147" s="2"/>
     </row>
-    <row r="148" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -5245,7 +5674,7 @@
       <c r="P148" s="2"/>
       <c r="Q148" s="2"/>
     </row>
-    <row r="149" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -5264,7 +5693,7 @@
       <c r="P149" s="2"/>
       <c r="Q149" s="2"/>
     </row>
-    <row r="150" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -5283,7 +5712,7 @@
       <c r="P150" s="2"/>
       <c r="Q150" s="2"/>
     </row>
-    <row r="151" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -5302,7 +5731,7 @@
       <c r="P151" s="2"/>
       <c r="Q151" s="2"/>
     </row>
-    <row r="152" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -5331,53 +5760,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.46484375" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>0.25</v>

</xml_diff>